<commit_message>
animatejs and graceful error handling with axios
</commit_message>
<xml_diff>
--- a/RBS_Uplift Training Schedule.xlsx
+++ b/RBS_Uplift Training Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chandan\e-learning\rbs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chandan\e-learning\rbs\source-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B139CC-6084-4F03-B332-CCB8F7EFFDAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB594917-4195-4FBD-9C86-D57DAA61294C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{5D1A0AA8-3127-4B7C-B042-AF2470C4840E}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{5D1A0AA8-3127-4B7C-B042-AF2470C4840E}"/>
   </bookViews>
   <sheets>
     <sheet name="Consolidate Schedule" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="350">
   <si>
     <t>Topic</t>
   </si>
@@ -1881,6 +1881,12 @@
   </si>
   <si>
     <t>Typescript</t>
+  </si>
+  <si>
+    <t>recap required?</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -4757,8 +4763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25C1995-8180-4701-9A49-D77C60B38FCE}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,10 +5821,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D27E392-10A9-46D0-9EAA-2310150A229D}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5828,7 +5834,7 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5841,8 +5847,11 @@
       <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -5856,7 +5865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -5870,7 +5879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -5884,7 +5893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -5898,7 +5907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -5912,7 +5921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5926,7 +5935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -5954,7 +5963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -5968,7 +5977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -5982,7 +5991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -5996,7 +6005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -6010,7 +6019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -6024,7 +6033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -6038,7 +6047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>219</v>
       </c>
@@ -6738,7 +6747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>220</v>
       </c>
@@ -6752,7 +6761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>221</v>
       </c>
@@ -6766,7 +6775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>222</v>
       </c>
@@ -6780,7 +6789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>223</v>
       </c>
@@ -6794,7 +6803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>224</v>
       </c>
@@ -6808,7 +6817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>225</v>
       </c>
@@ -6822,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>226</v>
       </c>
@@ -6836,7 +6845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>227</v>
       </c>
@@ -6850,7 +6859,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>228</v>
       </c>
@@ -6864,7 +6873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>229</v>
       </c>
@@ -6877,8 +6886,11 @@
       <c r="D75" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -6892,7 +6904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>231</v>
       </c>
@@ -6906,7 +6918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>232</v>
       </c>

</xml_diff>